<commit_message>
Add ADX jupyter book
</commit_message>
<xml_diff>
--- a/Forex investment forcast.xlsx
+++ b/Forex investment forcast.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ChanYong_Khaw\C drive\git\Trading_Study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2FCBD532-770D-4BF3-A8E5-8970F48522F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B42714-9F82-4407-836A-9D8A7FC7289C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8FF89886-3659-4EAC-B0B8-CFAEE3FA9B42}"/>
   </bookViews>
@@ -111,7 +111,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -121,6 +121,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CDF31E0-60DF-4495-9C84-DF5987AB436D}">
-  <dimension ref="D1:Q38"/>
+  <dimension ref="D1:R38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:Q39"/>
+    <sheetView tabSelected="1" topLeftCell="F8" zoomScale="145" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,8 +450,8 @@
     <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="10.7109375" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" customWidth="1"/>
     <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13.140625" bestFit="1" customWidth="1"/>
@@ -462,7 +463,7 @@
     <col min="28" max="29" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="4:18" x14ac:dyDescent="0.25">
       <c r="F1" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -470,7 +471,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="4" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>0</v>
       </c>
@@ -508,7 +509,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D5" s="2">
         <v>44480</v>
       </c>
@@ -520,11 +521,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G5">
-        <f>E5*F5</f>
+        <f t="shared" ref="G5:G38" si="0">E5*F5</f>
         <v>210.00000000000003</v>
       </c>
       <c r="H5">
-        <f>G5*4.1</f>
+        <f t="shared" ref="H5:H38" si="1">G5*4.1</f>
         <v>861</v>
       </c>
       <c r="L5" s="2">
@@ -538,37 +539,37 @@
         <v>0.08</v>
       </c>
       <c r="O5">
-        <f>M5*N5</f>
+        <f t="shared" ref="O5:O38" si="2">M5*N5</f>
         <v>240</v>
       </c>
       <c r="P5">
-        <f>O5*4.1</f>
+        <f t="shared" ref="P5:P38" si="3">O5*4.1</f>
         <v>983.99999999999989</v>
       </c>
     </row>
-    <row r="6" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D6" s="2">
         <f>D5+(5*7)</f>
         <v>44515</v>
       </c>
       <c r="E6" s="3">
-        <f>(INT(G5/100)*100)+E5</f>
+        <f t="shared" ref="E6:E38" si="4">(INT(G5/100)*100)+E5</f>
         <v>3200</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" ref="F6:F38" si="0">$F$1</f>
+        <f t="shared" ref="F6:F38" si="5">$F$1</f>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G6">
-        <f>E6*F6</f>
+        <f t="shared" si="0"/>
         <v>224.00000000000003</v>
       </c>
       <c r="H6">
-        <f>G6*4.1</f>
+        <f t="shared" si="1"/>
         <v>918.40000000000009</v>
       </c>
       <c r="I6">
-        <f>(E6-$M$5)*4.1</f>
+        <f t="shared" ref="I6:I38" si="6">(E6-$M$5)*4.1</f>
         <v>819.99999999999989</v>
       </c>
       <c r="L6" s="2">
@@ -576,19 +577,19 @@
         <v>44515</v>
       </c>
       <c r="M6" s="3">
-        <f>(INT(O5/100)*100)+M5</f>
+        <f t="shared" ref="M6:M38" si="7">(INT(O5/100)*100)+M5</f>
         <v>3200</v>
       </c>
       <c r="N6" s="1">
-        <f t="shared" ref="N6:N38" si="1">$N$1</f>
+        <f t="shared" ref="N6:N38" si="8">$N$1</f>
         <v>0.08</v>
       </c>
       <c r="O6">
-        <f>M6*N6</f>
+        <f t="shared" si="2"/>
         <v>256</v>
       </c>
       <c r="P6">
-        <f>O6*4.1</f>
+        <f t="shared" si="3"/>
         <v>1049.5999999999999</v>
       </c>
       <c r="Q6">
@@ -596,1604 +597,1610 @@
         <v>819.99999999999989</v>
       </c>
     </row>
-    <row r="7" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D7" s="2">
-        <f t="shared" ref="D7:D38" si="2">D6+(5*7)</f>
+        <f t="shared" ref="D7:D38" si="9">D6+(5*7)</f>
         <v>44550</v>
       </c>
       <c r="E7" s="3">
-        <f>(INT(G6/100)*100)+E6</f>
+        <f t="shared" si="4"/>
         <v>3400</v>
       </c>
       <c r="F7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G7">
-        <f>E7*F7</f>
+        <f t="shared" si="0"/>
         <v>238.00000000000003</v>
       </c>
       <c r="H7">
-        <f>G7*4.1</f>
+        <f t="shared" si="1"/>
         <v>975.80000000000007</v>
       </c>
       <c r="I7">
-        <f>(E7-$M$5)*4.1</f>
+        <f t="shared" si="6"/>
         <v>1639.9999999999998</v>
       </c>
       <c r="L7" s="2">
-        <f t="shared" ref="L7:L38" si="3">L6+(5*7)</f>
+        <f t="shared" ref="L7:L38" si="10">L6+(5*7)</f>
         <v>44550</v>
       </c>
       <c r="M7" s="3">
-        <f>(INT(O6/100)*100)+M6</f>
+        <f t="shared" si="7"/>
         <v>3400</v>
       </c>
       <c r="N7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0.08</v>
       </c>
       <c r="O7">
-        <f>M7*N7</f>
+        <f t="shared" si="2"/>
         <v>272</v>
       </c>
       <c r="P7">
-        <f>O7*4.1</f>
+        <f t="shared" si="3"/>
         <v>1115.1999999999998</v>
       </c>
       <c r="Q7">
-        <f t="shared" ref="Q7:Q38" si="4">(M7-$M$5)*4.1</f>
+        <f t="shared" ref="Q7:Q38" si="11">(M7-$M$5)*4.1</f>
         <v>1639.9999999999998</v>
       </c>
     </row>
-    <row r="8" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D8" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>44585</v>
       </c>
       <c r="E8" s="3">
-        <f>(INT(G7/100)*100)+E7</f>
+        <f t="shared" si="4"/>
         <v>3600</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G8">
-        <f>E8*F8</f>
+        <f t="shared" si="0"/>
         <v>252.00000000000003</v>
       </c>
       <c r="H8">
-        <f>G8*4.1</f>
+        <f t="shared" si="1"/>
         <v>1033.2</v>
       </c>
       <c r="I8">
-        <f>(E8-$M$5)*4.1</f>
+        <f t="shared" si="6"/>
         <v>2460</v>
       </c>
       <c r="L8" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>44585</v>
       </c>
       <c r="M8" s="3">
-        <f>(INT(O7/100)*100)+M7</f>
-        <v>3600</v>
+        <f>(INT(O7/100)*100)+M7+R8</f>
+        <v>4600</v>
       </c>
       <c r="N8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0.08</v>
       </c>
       <c r="O8">
-        <f>M8*N8</f>
-        <v>288</v>
+        <f t="shared" si="2"/>
+        <v>368</v>
       </c>
       <c r="P8">
-        <f>O8*4.1</f>
-        <v>1180.8</v>
+        <f t="shared" si="3"/>
+        <v>1508.8</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="4"/>
-        <v>2460</v>
-      </c>
-    </row>
-    <row r="9" spans="4:17" x14ac:dyDescent="0.25">
+        <f t="shared" si="11"/>
+        <v>6559.9999999999991</v>
+      </c>
+      <c r="R8">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D9" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>44620</v>
       </c>
       <c r="E9" s="3">
-        <f>(INT(G8/100)*100)+E8</f>
+        <f t="shared" si="4"/>
         <v>3800</v>
       </c>
       <c r="F9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G9">
-        <f>E9*F9</f>
+        <f t="shared" si="0"/>
         <v>266</v>
       </c>
       <c r="H9">
-        <f>G9*4.1</f>
+        <f t="shared" si="1"/>
         <v>1090.5999999999999</v>
       </c>
       <c r="I9">
-        <f>(E9-$M$5)*4.1</f>
+        <f t="shared" si="6"/>
         <v>3279.9999999999995</v>
       </c>
       <c r="L9" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>44620</v>
       </c>
       <c r="M9" s="3">
-        <f>(INT(O8/100)*100)+M8</f>
-        <v>3800</v>
+        <f t="shared" ref="M9:M38" si="12">(INT(O8/100)*100)+M8+R9</f>
+        <v>5900</v>
       </c>
       <c r="N9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0.08</v>
       </c>
       <c r="O9">
-        <f>M9*N9</f>
-        <v>304</v>
+        <f t="shared" si="2"/>
+        <v>472</v>
       </c>
       <c r="P9">
-        <f>O9*4.1</f>
-        <v>1246.3999999999999</v>
+        <f t="shared" si="3"/>
+        <v>1935.1999999999998</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="4"/>
-        <v>3279.9999999999995</v>
-      </c>
-    </row>
-    <row r="10" spans="4:17" x14ac:dyDescent="0.25">
+        <f t="shared" si="11"/>
+        <v>11889.999999999998</v>
+      </c>
+      <c r="R9">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D10" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>44655</v>
       </c>
       <c r="E10" s="3">
-        <f>(INT(G9/100)*100)+E9</f>
+        <f t="shared" si="4"/>
         <v>4000</v>
       </c>
       <c r="F10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G10">
-        <f>E10*F10</f>
+        <f t="shared" si="0"/>
         <v>280</v>
       </c>
       <c r="H10">
-        <f>G10*4.1</f>
+        <f t="shared" si="1"/>
         <v>1148</v>
       </c>
       <c r="I10">
-        <f>(E10-$M$5)*4.1</f>
+        <f t="shared" si="6"/>
         <v>4100</v>
       </c>
       <c r="L10" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>44655</v>
       </c>
       <c r="M10" s="3">
-        <f>(INT(O9/100)*100)+M9</f>
-        <v>4100</v>
+        <f t="shared" si="12"/>
+        <v>6300</v>
       </c>
       <c r="N10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0.08</v>
       </c>
       <c r="O10">
-        <f>M10*N10</f>
-        <v>328</v>
+        <f t="shared" si="2"/>
+        <v>504</v>
       </c>
       <c r="P10">
-        <f>O10*4.1</f>
-        <v>1344.8</v>
+        <f t="shared" si="3"/>
+        <v>2066.3999999999996</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="4"/>
-        <v>4510</v>
-      </c>
-    </row>
-    <row r="11" spans="4:17" x14ac:dyDescent="0.25">
+        <f t="shared" si="11"/>
+        <v>13529.999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D11" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>44690</v>
       </c>
       <c r="E11" s="3">
-        <f>(INT(G10/100)*100)+E10</f>
+        <f t="shared" si="4"/>
         <v>4200</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G11">
-        <f>E11*F11</f>
+        <f t="shared" si="0"/>
         <v>294</v>
       </c>
       <c r="H11">
-        <f>G11*4.1</f>
+        <f t="shared" si="1"/>
         <v>1205.3999999999999</v>
       </c>
       <c r="I11">
-        <f>(E11-$M$5)*4.1</f>
+        <f t="shared" si="6"/>
         <v>4920</v>
       </c>
       <c r="L11" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>44690</v>
       </c>
       <c r="M11" s="3">
-        <f>(INT(O10/100)*100)+M10</f>
+        <f t="shared" si="12"/>
+        <v>6800</v>
+      </c>
+      <c r="N11" s="1">
+        <f t="shared" si="8"/>
+        <v>0.08</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="2"/>
+        <v>544</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="3"/>
+        <v>2230.3999999999996</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="11"/>
+        <v>15579.999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D12" s="2">
+        <f t="shared" si="9"/>
+        <v>44725</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="4"/>
         <v>4400</v>
       </c>
-      <c r="N11" s="1">
-        <f t="shared" si="1"/>
-        <v>0.08</v>
-      </c>
-      <c r="O11">
-        <f>M11*N11</f>
-        <v>352</v>
-      </c>
-      <c r="P11">
-        <f>O11*4.1</f>
-        <v>1443.1999999999998</v>
-      </c>
-      <c r="Q11">
-        <f t="shared" si="4"/>
+      <c r="F12" s="1">
+        <f t="shared" si="5"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>308.00000000000006</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>1262.8000000000002</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="6"/>
         <v>5739.9999999999991</v>
       </c>
-    </row>
-    <row r="12" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D12" s="2">
-        <f t="shared" si="2"/>
+      <c r="L12" s="2">
+        <f t="shared" si="10"/>
         <v>44725</v>
       </c>
-      <c r="E12" s="3">
-        <f>(INT(G11/100)*100)+E11</f>
-        <v>4400</v>
-      </c>
-      <c r="F12" s="1">
-        <f t="shared" si="0"/>
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="G12">
-        <f>E12*F12</f>
-        <v>308.00000000000006</v>
-      </c>
-      <c r="H12">
-        <f>G12*4.1</f>
-        <v>1262.8000000000002</v>
-      </c>
-      <c r="I12">
-        <f>(E12-$M$5)*4.1</f>
-        <v>5739.9999999999991</v>
-      </c>
-      <c r="L12" s="2">
-        <f t="shared" si="3"/>
-        <v>44725</v>
-      </c>
       <c r="M12" s="3">
-        <f>(INT(O11/100)*100)+M11</f>
+        <f t="shared" si="12"/>
+        <v>7300</v>
+      </c>
+      <c r="N12" s="1">
+        <f t="shared" si="8"/>
+        <v>0.08</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="2"/>
+        <v>584</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="3"/>
+        <v>2394.3999999999996</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="11"/>
+        <v>17630</v>
+      </c>
+    </row>
+    <row r="13" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D13" s="2">
+        <f t="shared" si="9"/>
+        <v>44760</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="4"/>
         <v>4700</v>
       </c>
-      <c r="N12" s="1">
-        <f t="shared" si="1"/>
-        <v>0.08</v>
-      </c>
-      <c r="O12">
-        <f>M12*N12</f>
-        <v>376</v>
-      </c>
-      <c r="P12">
-        <f>O12*4.1</f>
-        <v>1541.6</v>
-      </c>
-      <c r="Q12">
-        <f t="shared" si="4"/>
+      <c r="F13" s="1">
+        <f t="shared" si="5"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>329.00000000000006</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>1348.9</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="6"/>
         <v>6969.9999999999991</v>
       </c>
-    </row>
-    <row r="13" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D13" s="2">
-        <f t="shared" si="2"/>
+      <c r="L13" s="2">
+        <f t="shared" si="10"/>
         <v>44760</v>
       </c>
-      <c r="E13" s="3">
-        <f>(INT(G12/100)*100)+E12</f>
-        <v>4700</v>
-      </c>
-      <c r="F13" s="1">
-        <f t="shared" si="0"/>
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="G13">
-        <f>E13*F13</f>
-        <v>329.00000000000006</v>
-      </c>
-      <c r="H13">
-        <f>G13*4.1</f>
-        <v>1348.9</v>
-      </c>
-      <c r="I13">
-        <f>(E13-$M$5)*4.1</f>
-        <v>6969.9999999999991</v>
-      </c>
-      <c r="L13" s="2">
-        <f t="shared" si="3"/>
-        <v>44760</v>
-      </c>
       <c r="M13" s="3">
-        <f>(INT(O12/100)*100)+M12</f>
+        <f t="shared" si="12"/>
+        <v>7800</v>
+      </c>
+      <c r="N13" s="1">
+        <f t="shared" si="8"/>
+        <v>0.08</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="2"/>
+        <v>624</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="3"/>
+        <v>2558.3999999999996</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="11"/>
+        <v>19680</v>
+      </c>
+    </row>
+    <row r="14" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D14" s="2">
+        <f t="shared" si="9"/>
+        <v>44795</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="4"/>
         <v>5000</v>
       </c>
-      <c r="N13" s="1">
-        <f t="shared" si="1"/>
-        <v>0.08</v>
-      </c>
-      <c r="O13">
-        <f>M13*N13</f>
-        <v>400</v>
-      </c>
-      <c r="P13">
-        <f>O13*4.1</f>
-        <v>1639.9999999999998</v>
-      </c>
-      <c r="Q13">
-        <f t="shared" si="4"/>
+      <c r="F14" s="1">
+        <f t="shared" si="5"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>350.00000000000006</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>1435</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="6"/>
         <v>8200</v>
       </c>
-    </row>
-    <row r="14" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D14" s="2">
-        <f t="shared" si="2"/>
+      <c r="L14" s="2">
+        <f t="shared" si="10"/>
         <v>44795</v>
       </c>
-      <c r="E14" s="3">
-        <f>(INT(G13/100)*100)+E13</f>
-        <v>5000</v>
-      </c>
-      <c r="F14" s="1">
-        <f t="shared" si="0"/>
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="G14">
-        <f>E14*F14</f>
-        <v>350.00000000000006</v>
-      </c>
-      <c r="H14">
-        <f>G14*4.1</f>
-        <v>1435</v>
-      </c>
-      <c r="I14">
-        <f>(E14-$M$5)*4.1</f>
-        <v>8200</v>
-      </c>
-      <c r="L14" s="2">
-        <f t="shared" si="3"/>
-        <v>44795</v>
-      </c>
       <c r="M14" s="3">
-        <f>(INT(O13/100)*100)+M13</f>
-        <v>5400</v>
+        <f t="shared" si="12"/>
+        <v>8400</v>
       </c>
       <c r="N14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0.08</v>
       </c>
       <c r="O14">
-        <f>M14*N14</f>
-        <v>432</v>
+        <f t="shared" si="2"/>
+        <v>672</v>
       </c>
       <c r="P14">
-        <f>O14*4.1</f>
-        <v>1771.1999999999998</v>
+        <f t="shared" si="3"/>
+        <v>2755.2</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="4"/>
-        <v>9840</v>
-      </c>
-    </row>
-    <row r="15" spans="4:17" x14ac:dyDescent="0.25">
+        <f t="shared" si="11"/>
+        <v>22139.999999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D15" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>44830</v>
       </c>
       <c r="E15" s="3">
-        <f>(INT(G14/100)*100)+E14</f>
+        <f t="shared" si="4"/>
         <v>5300</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G15">
-        <f>E15*F15</f>
+        <f t="shared" si="0"/>
         <v>371.00000000000006</v>
       </c>
       <c r="H15">
-        <f>G15*4.1</f>
+        <f t="shared" si="1"/>
         <v>1521.1000000000001</v>
       </c>
       <c r="I15">
-        <f>(E15-$M$5)*4.1</f>
+        <f t="shared" si="6"/>
         <v>9430</v>
       </c>
       <c r="L15" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>44830</v>
       </c>
-      <c r="M15" s="4">
-        <f>(INT(O14/100)*100)+M14</f>
-        <v>5800</v>
+      <c r="M15" s="9">
+        <f>(INT(O14/100)*100)+M14+R15</f>
+        <v>9000</v>
       </c>
       <c r="N15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0.08</v>
       </c>
       <c r="O15">
-        <f>M15*N15</f>
-        <v>464</v>
+        <f t="shared" si="2"/>
+        <v>720</v>
       </c>
       <c r="P15">
-        <f>O15*4.1</f>
-        <v>1902.3999999999999</v>
+        <f t="shared" si="3"/>
+        <v>2951.9999999999995</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="4"/>
-        <v>11479.999999999998</v>
-      </c>
-    </row>
-    <row r="16" spans="4:17" x14ac:dyDescent="0.25">
+        <f t="shared" si="11"/>
+        <v>24599.999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D16" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>44865</v>
       </c>
       <c r="E16" s="3">
-        <f>(INT(G15/100)*100)+E15</f>
+        <f t="shared" si="4"/>
         <v>5600</v>
       </c>
       <c r="F16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G16">
-        <f>E16*F16</f>
+        <f t="shared" si="0"/>
         <v>392.00000000000006</v>
       </c>
       <c r="H16">
-        <f>G16*4.1</f>
+        <f t="shared" si="1"/>
         <v>1607.2</v>
       </c>
       <c r="I16">
-        <f>(E16-$M$5)*4.1</f>
+        <f t="shared" si="6"/>
         <v>10659.999999999998</v>
       </c>
       <c r="L16" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>44865</v>
       </c>
-      <c r="M16" s="4">
-        <f>(INT(O15/100)*100)+M15</f>
-        <v>6200</v>
+      <c r="M16" s="9">
+        <f t="shared" si="12"/>
+        <v>9700</v>
       </c>
       <c r="N16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0.08</v>
       </c>
       <c r="O16">
-        <f>M16*N16</f>
-        <v>496</v>
+        <f t="shared" si="2"/>
+        <v>776</v>
       </c>
       <c r="P16">
-        <f>O16*4.1</f>
-        <v>2033.6</v>
+        <f t="shared" si="3"/>
+        <v>3181.6</v>
       </c>
       <c r="Q16">
-        <f t="shared" si="4"/>
-        <v>13119.999999999998</v>
+        <f t="shared" si="11"/>
+        <v>27469.999999999996</v>
       </c>
     </row>
     <row r="17" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D17" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>44900</v>
       </c>
       <c r="E17" s="3">
-        <f>(INT(G16/100)*100)+E16</f>
+        <f t="shared" si="4"/>
         <v>5900</v>
       </c>
       <c r="F17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G17">
-        <f>E17*F17</f>
+        <f t="shared" si="0"/>
         <v>413.00000000000006</v>
       </c>
       <c r="H17">
-        <f>G17*4.1</f>
+        <f t="shared" si="1"/>
         <v>1693.3000000000002</v>
       </c>
       <c r="I17">
-        <f>(E17-$M$5)*4.1</f>
+        <f t="shared" si="6"/>
         <v>11889.999999999998</v>
       </c>
       <c r="L17" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>44900</v>
       </c>
-      <c r="M17" s="4">
-        <f>(INT(O16/100)*100)+M16</f>
-        <v>6600</v>
+      <c r="M17" s="9">
+        <f t="shared" si="12"/>
+        <v>10400</v>
       </c>
       <c r="N17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0.08</v>
       </c>
       <c r="O17">
-        <f>M17*N17</f>
-        <v>528</v>
+        <f t="shared" si="2"/>
+        <v>832</v>
       </c>
       <c r="P17">
-        <f>O17*4.1</f>
-        <v>2164.7999999999997</v>
+        <f t="shared" si="3"/>
+        <v>3411.2</v>
       </c>
       <c r="Q17">
-        <f t="shared" si="4"/>
-        <v>14759.999999999998</v>
+        <f t="shared" si="11"/>
+        <v>30339.999999999996</v>
       </c>
     </row>
     <row r="18" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D18" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>44935</v>
       </c>
       <c r="E18" s="4">
-        <f>(INT(G17/100)*100)+E17</f>
+        <f t="shared" si="4"/>
         <v>6300</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G18">
-        <f>E18*F18</f>
+        <f t="shared" si="0"/>
         <v>441.00000000000006</v>
       </c>
       <c r="H18">
-        <f>G18*4.1</f>
+        <f t="shared" si="1"/>
         <v>1808.1000000000001</v>
       </c>
       <c r="I18">
-        <f>(E18-$M$5)*4.1</f>
+        <f t="shared" si="6"/>
         <v>13529.999999999998</v>
       </c>
       <c r="L18" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>44935</v>
       </c>
-      <c r="M18" s="4">
-        <f>(INT(O17/100)*100)+M17</f>
-        <v>7100</v>
+      <c r="M18" s="9">
+        <f t="shared" si="12"/>
+        <v>11200</v>
       </c>
       <c r="N18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0.08</v>
       </c>
       <c r="O18">
-        <f>M18*N18</f>
-        <v>568</v>
+        <f t="shared" si="2"/>
+        <v>896</v>
       </c>
       <c r="P18">
-        <f>O18*4.1</f>
-        <v>2328.7999999999997</v>
+        <f t="shared" si="3"/>
+        <v>3673.5999999999995</v>
       </c>
       <c r="Q18">
-        <f t="shared" si="4"/>
-        <v>16810</v>
+        <f t="shared" si="11"/>
+        <v>33620</v>
       </c>
     </row>
     <row r="19" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D19" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>44970</v>
       </c>
       <c r="E19" s="4">
-        <f>(INT(G18/100)*100)+E18</f>
+        <f t="shared" si="4"/>
         <v>6700</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G19">
-        <f>E19*F19</f>
+        <f t="shared" si="0"/>
         <v>469.00000000000006</v>
       </c>
       <c r="H19">
-        <f>G19*4.1</f>
+        <f t="shared" si="1"/>
         <v>1922.9</v>
       </c>
       <c r="I19">
-        <f>(E19-$M$5)*4.1</f>
+        <f t="shared" si="6"/>
         <v>15169.999999999998</v>
       </c>
       <c r="L19" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>44970</v>
       </c>
-      <c r="M19" s="4">
-        <f>(INT(O18/100)*100)+M18</f>
-        <v>7600</v>
+      <c r="M19" s="9">
+        <f t="shared" si="12"/>
+        <v>12000</v>
       </c>
       <c r="N19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0.08</v>
       </c>
       <c r="O19">
-        <f>M19*N19</f>
-        <v>608</v>
+        <f t="shared" si="2"/>
+        <v>960</v>
       </c>
       <c r="P19">
-        <f>O19*4.1</f>
-        <v>2492.7999999999997</v>
+        <f t="shared" si="3"/>
+        <v>3935.9999999999995</v>
       </c>
       <c r="Q19">
-        <f t="shared" si="4"/>
-        <v>18860</v>
+        <f t="shared" si="11"/>
+        <v>36900</v>
       </c>
     </row>
     <row r="20" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D20" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>45005</v>
       </c>
       <c r="E20" s="4">
-        <f>(INT(G19/100)*100)+E19</f>
+        <f t="shared" si="4"/>
         <v>7100</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G20">
-        <f>E20*F20</f>
+        <f t="shared" si="0"/>
         <v>497.00000000000006</v>
       </c>
       <c r="H20">
-        <f>G20*4.1</f>
+        <f t="shared" si="1"/>
         <v>2037.7</v>
       </c>
       <c r="I20">
-        <f>(E20-$M$5)*4.1</f>
+        <f t="shared" si="6"/>
         <v>16810</v>
       </c>
       <c r="L20" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45005</v>
       </c>
-      <c r="M20" s="4">
-        <f>(INT(O19/100)*100)+M19</f>
-        <v>8200</v>
+      <c r="M20" s="9">
+        <f t="shared" si="12"/>
+        <v>12900</v>
       </c>
       <c r="N20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0.08</v>
       </c>
       <c r="O20">
-        <f>M20*N20</f>
-        <v>656</v>
+        <f t="shared" si="2"/>
+        <v>1032</v>
       </c>
       <c r="P20">
-        <f>O20*4.1</f>
-        <v>2689.6</v>
+        <f t="shared" si="3"/>
+        <v>4231.2</v>
       </c>
       <c r="Q20">
-        <f t="shared" si="4"/>
-        <v>21319.999999999996</v>
+        <f t="shared" si="11"/>
+        <v>40590</v>
       </c>
     </row>
     <row r="21" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D21" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>45040</v>
       </c>
       <c r="E21" s="4">
-        <f>(INT(G20/100)*100)+E20</f>
+        <f t="shared" si="4"/>
         <v>7500</v>
       </c>
       <c r="F21" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G21">
-        <f>E21*F21</f>
+        <f t="shared" si="0"/>
         <v>525</v>
       </c>
       <c r="H21">
-        <f>G21*4.1</f>
+        <f t="shared" si="1"/>
         <v>2152.5</v>
       </c>
       <c r="I21">
-        <f>(E21-$M$5)*4.1</f>
+        <f t="shared" si="6"/>
         <v>18450</v>
       </c>
       <c r="L21" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45040</v>
       </c>
-      <c r="M21" s="4">
-        <f>(INT(O20/100)*100)+M20</f>
-        <v>8800</v>
+      <c r="M21" s="9">
+        <f t="shared" si="12"/>
+        <v>13900</v>
       </c>
       <c r="N21" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0.08</v>
       </c>
       <c r="O21">
-        <f>M21*N21</f>
-        <v>704</v>
+        <f t="shared" si="2"/>
+        <v>1112</v>
       </c>
       <c r="P21">
-        <f>O21*4.1</f>
-        <v>2886.3999999999996</v>
+        <f t="shared" si="3"/>
+        <v>4559.2</v>
       </c>
       <c r="Q21">
-        <f t="shared" si="4"/>
-        <v>23779.999999999996</v>
+        <f t="shared" si="11"/>
+        <v>44689.999999999993</v>
       </c>
     </row>
     <row r="22" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D22" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>45075</v>
       </c>
       <c r="E22" s="4">
-        <f>(INT(G21/100)*100)+E21</f>
+        <f t="shared" si="4"/>
         <v>8000</v>
       </c>
       <c r="F22" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G22">
-        <f>E22*F22</f>
+        <f t="shared" si="0"/>
         <v>560</v>
       </c>
       <c r="H22">
-        <f>G22*4.1</f>
+        <f t="shared" si="1"/>
         <v>2296</v>
       </c>
       <c r="I22">
-        <f>(E22-$M$5)*4.1</f>
+        <f t="shared" si="6"/>
         <v>20500</v>
       </c>
       <c r="L22" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45075</v>
       </c>
-      <c r="M22" s="4">
-        <f>(INT(O21/100)*100)+M21</f>
-        <v>9500</v>
+      <c r="M22" s="9">
+        <f t="shared" si="12"/>
+        <v>15000</v>
       </c>
       <c r="N22" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0.08</v>
       </c>
       <c r="O22">
-        <f>M22*N22</f>
-        <v>760</v>
+        <f t="shared" si="2"/>
+        <v>1200</v>
       </c>
       <c r="P22">
-        <f>O22*4.1</f>
-        <v>3115.9999999999995</v>
+        <f t="shared" si="3"/>
+        <v>4920</v>
       </c>
       <c r="Q22">
-        <f t="shared" si="4"/>
-        <v>26649.999999999996</v>
+        <f t="shared" si="11"/>
+        <v>49199.999999999993</v>
       </c>
     </row>
     <row r="23" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D23" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>45110</v>
       </c>
       <c r="E23" s="4">
-        <f>(INT(G22/100)*100)+E22</f>
+        <f t="shared" si="4"/>
         <v>8500</v>
       </c>
       <c r="F23" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G23">
-        <f>E23*F23</f>
+        <f t="shared" si="0"/>
         <v>595</v>
       </c>
       <c r="H23">
-        <f>G23*4.1</f>
+        <f t="shared" si="1"/>
         <v>2439.5</v>
       </c>
       <c r="I23">
-        <f>(E23-$M$5)*4.1</f>
+        <f t="shared" si="6"/>
         <v>22549.999999999996</v>
       </c>
       <c r="L23" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45110</v>
       </c>
-      <c r="M23" s="4">
-        <f>(INT(O22/100)*100)+M22</f>
-        <v>10200</v>
+      <c r="M23" s="9">
+        <f t="shared" si="12"/>
+        <v>16200</v>
       </c>
       <c r="N23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0.08</v>
       </c>
       <c r="O23">
-        <f>M23*N23</f>
-        <v>816</v>
+        <f t="shared" si="2"/>
+        <v>1296</v>
       </c>
       <c r="P23">
-        <f>O23*4.1</f>
-        <v>3345.6</v>
+        <f t="shared" si="3"/>
+        <v>5313.5999999999995</v>
       </c>
       <c r="Q23">
-        <f t="shared" si="4"/>
-        <v>29519.999999999996</v>
+        <f t="shared" si="11"/>
+        <v>54119.999999999993</v>
       </c>
     </row>
     <row r="24" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D24" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>45145</v>
       </c>
       <c r="E24" s="4">
-        <f>(INT(G23/100)*100)+E23</f>
+        <f t="shared" si="4"/>
         <v>9000</v>
       </c>
       <c r="F24" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G24">
-        <f>E24*F24</f>
+        <f t="shared" si="0"/>
         <v>630.00000000000011</v>
       </c>
       <c r="H24">
-        <f>G24*4.1</f>
+        <f t="shared" si="1"/>
         <v>2583.0000000000005</v>
       </c>
       <c r="I24">
-        <f>(E24-$M$5)*4.1</f>
+        <f t="shared" si="6"/>
         <v>24599.999999999996</v>
       </c>
       <c r="L24" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45145</v>
       </c>
-      <c r="M24" s="4">
-        <f>(INT(O23/100)*100)+M23</f>
-        <v>11000</v>
+      <c r="M24" s="9">
+        <f t="shared" si="12"/>
+        <v>17400</v>
       </c>
       <c r="N24" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0.08</v>
       </c>
       <c r="O24">
-        <f>M24*N24</f>
-        <v>880</v>
+        <f t="shared" si="2"/>
+        <v>1392</v>
       </c>
       <c r="P24">
-        <f>O24*4.1</f>
-        <v>3607.9999999999995</v>
+        <f t="shared" si="3"/>
+        <v>5707.2</v>
       </c>
       <c r="Q24">
-        <f t="shared" si="4"/>
-        <v>32800</v>
+        <f t="shared" si="11"/>
+        <v>59039.999999999993</v>
       </c>
     </row>
     <row r="25" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D25" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>45180</v>
       </c>
       <c r="E25" s="4">
-        <f>(INT(G24/100)*100)+E24</f>
+        <f t="shared" si="4"/>
         <v>9600</v>
       </c>
       <c r="F25" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G25">
-        <f>E25*F25</f>
+        <f t="shared" si="0"/>
         <v>672.00000000000011</v>
       </c>
       <c r="H25">
-        <f>G25*4.1</f>
+        <f t="shared" si="1"/>
         <v>2755.2000000000003</v>
       </c>
       <c r="I25">
-        <f>(E25-$M$5)*4.1</f>
+        <f t="shared" si="6"/>
         <v>27059.999999999996</v>
       </c>
       <c r="L25" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45180</v>
       </c>
-      <c r="M25" s="4">
-        <f>(INT(O24/100)*100)+M24</f>
-        <v>11800</v>
+      <c r="M25" s="9">
+        <f t="shared" si="12"/>
+        <v>18700</v>
       </c>
       <c r="N25" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0.08</v>
       </c>
       <c r="O25">
-        <f>M25*N25</f>
-        <v>944</v>
+        <f t="shared" si="2"/>
+        <v>1496</v>
       </c>
       <c r="P25">
-        <f>O25*4.1</f>
-        <v>3870.3999999999996</v>
+        <f t="shared" si="3"/>
+        <v>6133.5999999999995</v>
       </c>
       <c r="Q25">
-        <f t="shared" si="4"/>
-        <v>36080</v>
+        <f t="shared" si="11"/>
+        <v>64369.999999999993</v>
       </c>
     </row>
     <row r="26" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D26" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>45215</v>
       </c>
       <c r="E26" s="4">
-        <f>(INT(G25/100)*100)+E25</f>
+        <f t="shared" si="4"/>
         <v>10200</v>
       </c>
       <c r="F26" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G26">
-        <f>E26*F26</f>
+        <f t="shared" si="0"/>
         <v>714.00000000000011</v>
       </c>
       <c r="H26">
-        <f>G26*4.1</f>
+        <f t="shared" si="1"/>
         <v>2927.4</v>
       </c>
       <c r="I26">
-        <f>(E26-$M$5)*4.1</f>
+        <f t="shared" si="6"/>
         <v>29519.999999999996</v>
       </c>
       <c r="L26" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45215</v>
       </c>
-      <c r="M26" s="4">
-        <f>(INT(O25/100)*100)+M25</f>
-        <v>12700</v>
+      <c r="M26" s="9">
+        <f t="shared" si="12"/>
+        <v>20100</v>
       </c>
       <c r="N26" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0.08</v>
       </c>
       <c r="O26">
-        <f>M26*N26</f>
-        <v>1016</v>
+        <f t="shared" si="2"/>
+        <v>1608</v>
       </c>
       <c r="P26">
-        <f>O26*4.1</f>
-        <v>4165.5999999999995</v>
+        <f t="shared" si="3"/>
+        <v>6592.7999999999993</v>
       </c>
       <c r="Q26">
-        <f t="shared" si="4"/>
-        <v>39770</v>
+        <f t="shared" si="11"/>
+        <v>70110</v>
       </c>
     </row>
     <row r="27" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D27" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>45250</v>
       </c>
       <c r="E27" s="4">
-        <f>(INT(G26/100)*100)+E26</f>
+        <f t="shared" si="4"/>
         <v>10900</v>
       </c>
       <c r="F27" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G27">
-        <f>E27*F27</f>
+        <f t="shared" si="0"/>
         <v>763.00000000000011</v>
       </c>
       <c r="H27">
-        <f>G27*4.1</f>
+        <f t="shared" si="1"/>
         <v>3128.3</v>
       </c>
       <c r="I27">
-        <f>(E27-$M$5)*4.1</f>
+        <f t="shared" si="6"/>
         <v>32389.999999999996</v>
       </c>
       <c r="L27" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45250</v>
       </c>
-      <c r="M27" s="4">
-        <f>(INT(O26/100)*100)+M26</f>
-        <v>13700</v>
+      <c r="M27" s="9">
+        <f t="shared" si="12"/>
+        <v>21700</v>
       </c>
       <c r="N27" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0.08</v>
       </c>
       <c r="O27">
-        <f>M27*N27</f>
-        <v>1096</v>
+        <f t="shared" si="2"/>
+        <v>1736</v>
       </c>
       <c r="P27">
-        <f>O27*4.1</f>
-        <v>4493.5999999999995</v>
+        <f t="shared" si="3"/>
+        <v>7117.5999999999995</v>
       </c>
       <c r="Q27">
-        <f t="shared" si="4"/>
-        <v>43869.999999999993</v>
+        <f t="shared" si="11"/>
+        <v>76670</v>
       </c>
     </row>
     <row r="28" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D28" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>45285</v>
       </c>
       <c r="E28" s="4">
-        <f>(INT(G27/100)*100)+E27</f>
+        <f t="shared" si="4"/>
         <v>11600</v>
       </c>
       <c r="F28" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G28">
-        <f>E28*F28</f>
+        <f t="shared" si="0"/>
         <v>812.00000000000011</v>
       </c>
       <c r="H28">
-        <f>G28*4.1</f>
+        <f t="shared" si="1"/>
         <v>3329.2000000000003</v>
       </c>
       <c r="I28">
-        <f>(E28-$M$5)*4.1</f>
+        <f t="shared" si="6"/>
         <v>35260</v>
       </c>
       <c r="L28" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45285</v>
       </c>
-      <c r="M28" s="4">
-        <f>(INT(O27/100)*100)+M27</f>
-        <v>14700</v>
+      <c r="M28" s="9">
+        <f t="shared" si="12"/>
+        <v>23400</v>
       </c>
       <c r="N28" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0.08</v>
       </c>
       <c r="O28">
-        <f>M28*N28</f>
-        <v>1176</v>
+        <f t="shared" si="2"/>
+        <v>1872</v>
       </c>
       <c r="P28">
-        <f>O28*4.1</f>
-        <v>4821.5999999999995</v>
+        <f t="shared" si="3"/>
+        <v>7675.1999999999989</v>
       </c>
       <c r="Q28">
-        <f t="shared" si="4"/>
-        <v>47969.999999999993</v>
+        <f t="shared" si="11"/>
+        <v>83640</v>
       </c>
     </row>
     <row r="29" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D29" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>45320</v>
       </c>
       <c r="E29" s="4">
-        <f>(INT(G28/100)*100)+E28</f>
+        <f t="shared" si="4"/>
         <v>12400</v>
       </c>
       <c r="F29" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G29">
-        <f>E29*F29</f>
+        <f t="shared" si="0"/>
         <v>868.00000000000011</v>
       </c>
       <c r="H29">
-        <f>G29*4.1</f>
+        <f t="shared" si="1"/>
         <v>3558.8</v>
       </c>
       <c r="I29">
-        <f>(E29-$M$5)*4.1</f>
+        <f t="shared" si="6"/>
         <v>38540</v>
       </c>
       <c r="L29" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45320</v>
       </c>
-      <c r="M29" s="6">
-        <f>(INT(O28/100)*100)+M28</f>
-        <v>15800</v>
+      <c r="M29" s="3">
+        <f t="shared" si="12"/>
+        <v>25200</v>
       </c>
       <c r="N29" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0.08</v>
       </c>
       <c r="O29">
-        <f>M29*N29</f>
-        <v>1264</v>
+        <f t="shared" si="2"/>
+        <v>2016</v>
       </c>
       <c r="P29">
-        <f>O29*4.1</f>
-        <v>5182.3999999999996</v>
+        <f t="shared" si="3"/>
+        <v>8265.5999999999985</v>
       </c>
       <c r="Q29">
-        <f t="shared" si="4"/>
-        <v>52479.999999999993</v>
+        <f t="shared" si="11"/>
+        <v>91019.999999999985</v>
       </c>
     </row>
     <row r="30" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D30" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>45355</v>
       </c>
       <c r="E30" s="4">
-        <f>(INT(G29/100)*100)+E29</f>
+        <f t="shared" si="4"/>
         <v>13200</v>
       </c>
       <c r="F30" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G30">
-        <f>E30*F30</f>
+        <f t="shared" si="0"/>
         <v>924.00000000000011</v>
       </c>
       <c r="H30">
-        <f>G30*4.1</f>
+        <f t="shared" si="1"/>
         <v>3788.4</v>
       </c>
       <c r="I30">
-        <f>(E30-$M$5)*4.1</f>
+        <f t="shared" si="6"/>
         <v>41820</v>
       </c>
       <c r="L30" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45355</v>
       </c>
-      <c r="M30" s="6">
-        <f>(INT(O29/100)*100)+M29</f>
-        <v>17000</v>
+      <c r="M30" s="3">
+        <f t="shared" si="12"/>
+        <v>27200</v>
       </c>
       <c r="N30" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0.08</v>
       </c>
       <c r="O30">
-        <f>M30*N30</f>
-        <v>1360</v>
+        <f t="shared" si="2"/>
+        <v>2176</v>
       </c>
       <c r="P30">
-        <f>O30*4.1</f>
-        <v>5575.9999999999991</v>
+        <f t="shared" si="3"/>
+        <v>8921.5999999999985</v>
       </c>
       <c r="Q30">
-        <f t="shared" si="4"/>
-        <v>57399.999999999993</v>
+        <f t="shared" si="11"/>
+        <v>99219.999999999985</v>
       </c>
     </row>
     <row r="31" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D31" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>45390</v>
       </c>
       <c r="E31" s="4">
-        <f>(INT(G30/100)*100)+E30</f>
+        <f t="shared" si="4"/>
         <v>14100</v>
       </c>
       <c r="F31" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G31">
-        <f>E31*F31</f>
+        <f t="shared" si="0"/>
         <v>987.00000000000011</v>
       </c>
       <c r="H31">
-        <f>G31*4.1</f>
+        <f t="shared" si="1"/>
         <v>4046.7000000000003</v>
       </c>
       <c r="I31">
-        <f>(E31-$M$5)*4.1</f>
+        <f t="shared" si="6"/>
         <v>45509.999999999993</v>
       </c>
       <c r="L31" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45390</v>
       </c>
-      <c r="M31" s="6">
-        <f>(INT(O30/100)*100)+M30</f>
-        <v>18300</v>
+      <c r="M31" s="3">
+        <f t="shared" si="12"/>
+        <v>29300</v>
       </c>
       <c r="N31" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0.08</v>
       </c>
       <c r="O31">
-        <f>M31*N31</f>
-        <v>1464</v>
+        <f t="shared" si="2"/>
+        <v>2344</v>
       </c>
       <c r="P31">
-        <f>O31*4.1</f>
-        <v>6002.4</v>
+        <f t="shared" si="3"/>
+        <v>9610.4</v>
       </c>
       <c r="Q31">
-        <f t="shared" si="4"/>
-        <v>62729.999999999993</v>
+        <f t="shared" si="11"/>
+        <v>107829.99999999999</v>
       </c>
     </row>
     <row r="32" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>45425</v>
       </c>
       <c r="E32" s="4">
-        <f>(INT(G31/100)*100)+E31</f>
+        <f t="shared" si="4"/>
         <v>15000</v>
       </c>
       <c r="F32" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G32">
-        <f>E32*F32</f>
+        <f t="shared" si="0"/>
         <v>1050</v>
       </c>
       <c r="H32">
-        <f>G32*4.1</f>
+        <f t="shared" si="1"/>
         <v>4305</v>
       </c>
       <c r="I32">
-        <f>(E32-$M$5)*4.1</f>
+        <f t="shared" si="6"/>
         <v>49199.999999999993</v>
       </c>
       <c r="L32" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45425</v>
       </c>
-      <c r="M32" s="6">
-        <f>(INT(O31/100)*100)+M31</f>
-        <v>19700</v>
+      <c r="M32" s="3">
+        <f t="shared" si="12"/>
+        <v>31600</v>
       </c>
       <c r="N32" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0.08</v>
       </c>
       <c r="O32">
-        <f>M32*N32</f>
-        <v>1576</v>
+        <f t="shared" si="2"/>
+        <v>2528</v>
       </c>
       <c r="P32">
-        <f>O32*4.1</f>
-        <v>6461.5999999999995</v>
+        <f t="shared" si="3"/>
+        <v>10364.799999999999</v>
       </c>
       <c r="Q32">
-        <f t="shared" si="4"/>
-        <v>68470</v>
+        <f t="shared" si="11"/>
+        <v>117259.99999999999</v>
       </c>
     </row>
     <row r="33" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D33" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>45460</v>
       </c>
       <c r="E33" s="4">
-        <f>(INT(G32/100)*100)+E32</f>
+        <f t="shared" si="4"/>
         <v>16000</v>
       </c>
       <c r="F33" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G33">
-        <f>E33*F33</f>
+        <f t="shared" si="0"/>
         <v>1120</v>
       </c>
       <c r="H33">
-        <f>G33*4.1</f>
+        <f t="shared" si="1"/>
         <v>4592</v>
       </c>
       <c r="I33">
-        <f>(E33-$M$5)*4.1</f>
+        <f t="shared" si="6"/>
         <v>53299.999999999993</v>
       </c>
       <c r="L33" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45460</v>
       </c>
-      <c r="M33" s="6">
-        <f>(INT(O32/100)*100)+M32</f>
-        <v>21200</v>
+      <c r="M33" s="3">
+        <f t="shared" si="12"/>
+        <v>34100</v>
       </c>
       <c r="N33" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0.08</v>
       </c>
       <c r="O33">
-        <f>M33*N33</f>
-        <v>1696</v>
+        <f t="shared" si="2"/>
+        <v>2728</v>
       </c>
       <c r="P33">
-        <f>O33*4.1</f>
-        <v>6953.5999999999995</v>
+        <f t="shared" si="3"/>
+        <v>11184.8</v>
       </c>
       <c r="Q33">
-        <f t="shared" si="4"/>
-        <v>74620</v>
+        <f t="shared" si="11"/>
+        <v>127509.99999999999</v>
       </c>
     </row>
     <row r="34" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D34" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>45495</v>
       </c>
       <c r="E34" s="4">
-        <f>(INT(G33/100)*100)+E33</f>
+        <f t="shared" si="4"/>
         <v>17100</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G34">
-        <f>E34*F34</f>
+        <f t="shared" si="0"/>
         <v>1197.0000000000002</v>
       </c>
       <c r="H34">
-        <f>G34*4.1</f>
+        <f t="shared" si="1"/>
         <v>4907.7000000000007</v>
       </c>
       <c r="I34">
-        <f>(E34-$M$5)*4.1</f>
+        <f t="shared" si="6"/>
         <v>57809.999999999993</v>
       </c>
       <c r="L34" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45495</v>
       </c>
-      <c r="M34" s="6">
-        <f>(INT(O33/100)*100)+M33</f>
-        <v>22800</v>
+      <c r="M34" s="3">
+        <f t="shared" si="12"/>
+        <v>36800</v>
       </c>
       <c r="N34" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0.08</v>
       </c>
       <c r="O34">
-        <f>M34*N34</f>
-        <v>1824</v>
+        <f t="shared" si="2"/>
+        <v>2944</v>
       </c>
       <c r="P34">
-        <f>O34*4.1</f>
-        <v>7478.4</v>
+        <f t="shared" si="3"/>
+        <v>12070.4</v>
       </c>
       <c r="Q34">
-        <f t="shared" si="4"/>
-        <v>81180</v>
+        <f t="shared" si="11"/>
+        <v>138580</v>
       </c>
     </row>
     <row r="35" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D35" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>45530</v>
       </c>
       <c r="E35" s="6">
-        <f>(INT(G34/100)*100)+E34</f>
+        <f t="shared" si="4"/>
         <v>18200</v>
       </c>
       <c r="F35" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G35">
-        <f>E35*F35</f>
+        <f t="shared" si="0"/>
         <v>1274.0000000000002</v>
       </c>
       <c r="H35">
-        <f>G35*4.1</f>
+        <f t="shared" si="1"/>
         <v>5223.4000000000005</v>
       </c>
       <c r="I35">
-        <f>(E35-$M$5)*4.1</f>
+        <f t="shared" si="6"/>
         <v>62319.999999999993</v>
       </c>
       <c r="L35" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45530</v>
       </c>
-      <c r="M35" s="6">
-        <f>(INT(O34/100)*100)+M34</f>
-        <v>24600</v>
+      <c r="M35" s="3">
+        <f t="shared" si="12"/>
+        <v>39700</v>
       </c>
       <c r="N35" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0.08</v>
       </c>
       <c r="O35">
-        <f>M35*N35</f>
-        <v>1968</v>
+        <f t="shared" si="2"/>
+        <v>3176</v>
       </c>
       <c r="P35">
-        <f>O35*4.1</f>
-        <v>8068.7999999999993</v>
+        <f t="shared" si="3"/>
+        <v>13021.599999999999</v>
       </c>
       <c r="Q35">
-        <f t="shared" si="4"/>
-        <v>88559.999999999985</v>
+        <f t="shared" si="11"/>
+        <v>150470</v>
       </c>
     </row>
     <row r="36" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D36" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>45565</v>
       </c>
       <c r="E36" s="6">
-        <f>(INT(G35/100)*100)+E35</f>
+        <f t="shared" si="4"/>
         <v>19400</v>
       </c>
       <c r="F36" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G36">
-        <f>E36*F36</f>
+        <f t="shared" si="0"/>
         <v>1358.0000000000002</v>
       </c>
       <c r="H36">
-        <f>G36*4.1</f>
+        <f t="shared" si="1"/>
         <v>5567.8</v>
       </c>
       <c r="I36">
-        <f>(E36-$M$5)*4.1</f>
+        <f t="shared" si="6"/>
         <v>67240</v>
       </c>
       <c r="L36" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45565</v>
       </c>
-      <c r="M36" s="6">
-        <f>(INT(O35/100)*100)+M35</f>
-        <v>26500</v>
+      <c r="M36" s="3">
+        <f t="shared" si="12"/>
+        <v>42800</v>
       </c>
       <c r="N36" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0.08</v>
       </c>
       <c r="O36">
-        <f>M36*N36</f>
-        <v>2120</v>
+        <f t="shared" si="2"/>
+        <v>3424</v>
       </c>
       <c r="P36">
-        <f>O36*4.1</f>
-        <v>8692</v>
+        <f t="shared" si="3"/>
+        <v>14038.4</v>
       </c>
       <c r="Q36">
-        <f t="shared" si="4"/>
-        <v>96349.999999999985</v>
+        <f t="shared" si="11"/>
+        <v>163180</v>
       </c>
     </row>
     <row r="37" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D37" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>45600</v>
       </c>
       <c r="E37" s="6">
-        <f>(INT(G36/100)*100)+E36</f>
+        <f t="shared" si="4"/>
         <v>20700</v>
       </c>
       <c r="F37" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G37">
-        <f>E37*F37</f>
+        <f t="shared" si="0"/>
         <v>1449.0000000000002</v>
       </c>
       <c r="H37">
-        <f>G37*4.1</f>
+        <f t="shared" si="1"/>
         <v>5940.9000000000005</v>
       </c>
       <c r="I37">
-        <f>(E37-$M$5)*4.1</f>
+        <f t="shared" si="6"/>
         <v>72570</v>
       </c>
       <c r="L37" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45600</v>
       </c>
-      <c r="M37" s="6">
-        <f>(INT(O36/100)*100)+M36</f>
-        <v>28600</v>
+      <c r="M37" s="3">
+        <f t="shared" si="12"/>
+        <v>46200</v>
       </c>
       <c r="N37" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0.08</v>
       </c>
       <c r="O37">
-        <f>M37*N37</f>
-        <v>2288</v>
+        <f t="shared" si="2"/>
+        <v>3696</v>
       </c>
       <c r="P37">
-        <f>O37*4.1</f>
-        <v>9380.7999999999993</v>
+        <f t="shared" si="3"/>
+        <v>15153.599999999999</v>
       </c>
       <c r="Q37">
-        <f t="shared" si="4"/>
-        <v>104959.99999999999</v>
+        <f t="shared" si="11"/>
+        <v>177119.99999999997</v>
       </c>
     </row>
     <row r="38" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D38" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>45635</v>
       </c>
       <c r="E38" s="6">
-        <f>(INT(G37/100)*100)+E37</f>
+        <f t="shared" si="4"/>
         <v>22100</v>
       </c>
       <c r="F38" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G38">
-        <f>E38*F38</f>
+        <f t="shared" si="0"/>
         <v>1547.0000000000002</v>
       </c>
       <c r="H38">
-        <f>G38*4.1</f>
+        <f t="shared" si="1"/>
         <v>6342.7000000000007</v>
       </c>
       <c r="I38">
-        <f>(E38-$M$5)*4.1</f>
+        <f t="shared" si="6"/>
         <v>78310</v>
       </c>
       <c r="L38" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45635</v>
       </c>
-      <c r="M38" s="6">
-        <f>(INT(O37/100)*100)+M37</f>
-        <v>30800</v>
+      <c r="M38" s="3">
+        <f t="shared" si="12"/>
+        <v>49800</v>
       </c>
       <c r="N38" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
         <v>0.08</v>
       </c>
       <c r="O38">
-        <f>M38*N38</f>
-        <v>2464</v>
+        <f t="shared" si="2"/>
+        <v>3984</v>
       </c>
       <c r="P38">
-        <f>O38*4.1</f>
-        <v>10102.4</v>
+        <f t="shared" si="3"/>
+        <v>16334.399999999998</v>
       </c>
       <c r="Q38">
-        <f t="shared" si="4"/>
-        <v>113979.99999999999</v>
+        <f t="shared" si="11"/>
+        <v>191879.99999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>